<commit_message>
Added weakly scalable graphs
</commit_message>
<xml_diff>
--- a/Timing_Data/Final Project 4F03 MPI times.xlsx
+++ b/Timing_Data/Final Project 4F03 MPI times.xlsx
@@ -38,7 +38,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -77,6 +77,21 @@
       <sz val="10"/>
       <color rgb="FF595959"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -178,7 +193,7 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFB3B3B3"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
@@ -190,7 +205,7 @@
       <rgbColor rgb="FFED7D31"/>
       <rgbColor rgb="FF595959"/>
       <rgbColor rgb="FFA5A5A5"/>
-      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF004586"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
@@ -736,11 +751,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="76319"/>
-        <c:axId val="67671343"/>
+        <c:axId val="31534707"/>
+        <c:axId val="7766575"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="76319"/>
+        <c:axId val="31534707"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -767,7 +782,7 @@
                     </a:solidFill>
                     <a:latin typeface="Calibri"/>
                   </a:rPr>
-                  <a:t>Processes</a:t>
+                  <a:t>Number of Processors</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -800,12 +815,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="67671343"/>
+        <c:crossAx val="7766575"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="67671343"/>
+        <c:axId val="7766575"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -875,7 +890,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="76319"/>
+        <c:crossAx val="31534707"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1460,11 +1475,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="61664847"/>
-        <c:axId val="97000532"/>
+        <c:axId val="39829716"/>
+        <c:axId val="77063726"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="61664847"/>
+        <c:axId val="39829716"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1491,7 +1506,7 @@
                     </a:solidFill>
                     <a:latin typeface="Calibri"/>
                   </a:rPr>
-                  <a:t>Processes</a:t>
+                  <a:t>Number of Processors</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1524,12 +1539,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97000532"/>
+        <c:crossAx val="77063726"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="97000532"/>
+        <c:axId val="77063726"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1599,7 +1614,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61664847"/>
+        <c:crossAx val="39829716"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2184,11 +2199,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="74604525"/>
-        <c:axId val="92029375"/>
+        <c:axId val="12551140"/>
+        <c:axId val="77776822"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="74604525"/>
+        <c:axId val="12551140"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2215,7 +2230,7 @@
                     </a:solidFill>
                     <a:latin typeface="Calibri"/>
                   </a:rPr>
-                  <a:t>Processes</a:t>
+                  <a:t>Number of Processors</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2248,12 +2263,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92029375"/>
+        <c:crossAx val="77776822"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="92029375"/>
+        <c:axId val="77776822"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2323,7 +2338,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74604525"/>
+        <c:crossAx val="12551140"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2375,6 +2390,264 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Weakly Scalable Plot for MPI Implementation</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2,Sheet1!$A$11,Sheet1!$A$20,Sheet1!$A$28,Sheet1!$A$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$2,Sheet1!$E$11,Sheet1!$E$20,Sheet1!$E$28,Sheet1!$E$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.484162895927602</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.253110419906687</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0981104651162791</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0704617834394904</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="686065"/>
+        <c:axId val="28097490"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="686065"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Number of Processors</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="28097490"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="28097490"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Efficiency</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="686065"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -2386,9 +2659,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>247320</xdr:colOff>
+      <xdr:colOff>246960</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>139320</xdr:rowOff>
+      <xdr:rowOff>138960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2397,7 +2670,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="5467320" y="266400"/>
-        <a:ext cx="5997600" cy="2920680"/>
+        <a:ext cx="5997240" cy="2920320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2416,9 +2689,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>247320</xdr:colOff>
+      <xdr:colOff>246960</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>88560</xdr:rowOff>
+      <xdr:rowOff>88200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2427,7 +2700,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="5727600" y="3644640"/>
-        <a:ext cx="5737320" cy="2742840"/>
+        <a:ext cx="5736960" cy="2742480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2446,9 +2719,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>615600</xdr:colOff>
+      <xdr:colOff>615240</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>151920</xdr:rowOff>
+      <xdr:rowOff>151560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2457,11 +2730,41 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="11662200" y="1803240"/>
-        <a:ext cx="5270040" cy="3022200"/>
+        <a:ext cx="5269680" cy="3021840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>951480</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>145080</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>588600</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>135360</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="12169080" y="5225040"/>
+        <a:ext cx="5756040" cy="3241440"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2478,7 +2781,7 @@
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N35" activeCellId="0" sqref="N35"/>
+      <selection pane="topLeft" activeCell="N26" activeCellId="0" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>